<commit_message>
Fixed erronous graphs and data
</commit_message>
<xml_diff>
--- a/Results/Excel/Overhead Ratio.xlsx
+++ b/Results/Excel/Overhead Ratio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver Mitchell\Documents\GitHub\MSci_DTNs_under_DOS\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver Mitchell\Documents\GitHub\MSci_DTNs_under_DOS\Results\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753D9C17-6E40-4F05-9AB9-9B32894DDA49}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E72932F-3B4B-4FA1-8A9F-D9477A366DF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1476" yWindow="0" windowWidth="22548" windowHeight="9576" tabRatio="766" xr2:uid="{5FA714C0-B773-4060-825F-1666625488FF}"/>
+    <workbookView xWindow="1968" yWindow="0" windowWidth="22548" windowHeight="9576" tabRatio="766" xr2:uid="{5FA714C0-B773-4060-825F-1666625488FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario 1" sheetId="1" r:id="rId1"/>
@@ -1565,16 +1565,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="1">
-                  <c:v>18.5</c:v>
+                  <c:v>59.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.3</c:v>
+                  <c:v>35.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.099999999999994</c:v>
+                  <c:v>33.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69.599999999999994</c:v>
+                  <c:v>40.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2065,16 +2065,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>18.5</c:v>
+                  <c:v>59.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.3</c:v>
+                  <c:v>35.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.099999999999994</c:v>
+                  <c:v>33.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69.599999999999994</c:v>
+                  <c:v>40.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3018,7 +3018,7 @@
         <c:crossAx val="464569184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="100"/>
+        <c:majorUnit val="20"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5422,8 +5422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A709C639-1991-4027-8842-E6C5F0991560}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5453,16 +5453,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>18.5</v>
+        <v>59.3</v>
       </c>
       <c r="D2">
-        <v>47.3</v>
+        <v>35.6</v>
       </c>
       <c r="E2">
-        <v>67.099999999999994</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="F2">
-        <v>69.599999999999994</v>
+        <v>40.1</v>
       </c>
       <c r="G2" s="1"/>
     </row>

</xml_diff>